<commit_message>
hyy add website investigation plan
</commit_message>
<xml_diff>
--- a/团队项目进度一览表.xlsx
+++ b/团队项目进度一览表.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouxingxing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\材料\足球圈\git\self-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,20 +18,20 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">任务!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
   <si>
     <t>任务列表</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -228,13 +228,16 @@
       <t>mo ban</t>
     </rPh>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://isl.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="13"/>
       <color theme="4" tint="0.39991454817346722"/>
@@ -670,68 +673,107 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -741,45 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1097,7 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
@@ -1107,20 +1110,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1131,7 @@
       <c r="D1" s="13"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7" ht="24.95" customHeight="1">
       <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1167,7 +1170,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7" ht="24.95" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1189,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7" ht="24.95" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1208,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7" ht="24.95" customHeight="1">
       <c r="F6" s="10">
         <f>--(Table1[[#This Row],[完成百分比]]&gt;=1)</f>
         <v>0</v>
@@ -1301,451 +1304,445 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="41"/>
-    <col min="2" max="2" width="11" style="29" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="31" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="29"/>
-    <col min="6" max="6" width="10.7109375" style="30"/>
-    <col min="7" max="7" width="19.5703125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="29"/>
-    <col min="9" max="9" width="10.7109375" style="30"/>
-    <col min="10" max="10" width="19.140625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="29"/>
-    <col min="12" max="12" width="10.7109375" style="30"/>
-    <col min="13" max="13" width="18.5703125" style="31" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="29"/>
-    <col min="15" max="15" width="10.7109375" style="30"/>
-    <col min="16" max="16" width="19.140625" style="31" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="29"/>
-    <col min="18" max="18" width="10.7109375" style="30"/>
-    <col min="19" max="19" width="19.28515625" style="31" customWidth="1"/>
-    <col min="20" max="16384" width="10.7109375" style="16"/>
+    <col min="1" max="1" width="10.6640625" style="32"/>
+    <col min="2" max="2" width="11" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="25"/>
+    <col min="6" max="6" width="10.6640625" style="26"/>
+    <col min="7" max="7" width="19.5546875" style="27" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="25"/>
+    <col min="9" max="9" width="10.6640625" style="26"/>
+    <col min="10" max="10" width="19.109375" style="27" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="25"/>
+    <col min="12" max="12" width="10.6640625" style="26"/>
+    <col min="13" max="13" width="18.5546875" style="27" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="25"/>
+    <col min="15" max="15" width="10.6640625" style="26"/>
+    <col min="16" max="16" width="19.109375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="25"/>
+    <col min="18" max="18" width="10.6640625" style="26"/>
+    <col min="19" max="19" width="19.33203125" style="27" customWidth="1"/>
+    <col min="20" max="16384" width="10.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="53" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52"/>
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:19" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="40"/>
+      <c r="B1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="38" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="38" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="38" t="s">
+      <c r="L1" s="52"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="39"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="38" t="s">
+      <c r="O1" s="52"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="39"/>
-      <c r="S1" s="40"/>
-    </row>
-    <row r="2" spans="1:19" ht="20" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="42" t="s">
+      <c r="R1" s="52"/>
+      <c r="S1" s="53"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickTop="1">
+      <c r="A2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="32" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="23" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="32" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="23" t="s">
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="32" t="s">
+      <c r="O2" s="46"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="33"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="42"/>
-      <c r="B3" s="25" t="s">
+      <c r="R2" s="43"/>
+      <c r="S2" s="44"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="49"/>
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="35" t="s">
+      <c r="S3" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="27">
+    <row r="4" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A4" s="50"/>
+      <c r="B4" s="23">
         <v>5.3</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <v>6.6</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="36">
+      <c r="E4" s="30">
+        <v>6.3</v>
+      </c>
+      <c r="F4" s="20">
+        <v>6.6</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="30">
         <v>6.1</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="20">
         <v>6.1</v>
       </c>
-      <c r="S4" s="37"/>
-    </row>
-    <row r="5" spans="1:19" s="50" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-    </row>
-    <row r="6" spans="1:19" ht="20" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="44" t="s">
+      <c r="S4" s="31"/>
+    </row>
+    <row r="5" spans="1:19" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickTop="1">
+      <c r="A6" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="32" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="33"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7" s="42"/>
-      <c r="B7" s="25" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="44"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="49"/>
+      <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="M7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="34" t="s">
+      <c r="Q7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="35" t="s">
+      <c r="S7" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="37"/>
-    </row>
-    <row r="9" spans="1:19" s="50" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-    </row>
-    <row r="10" spans="1:19" ht="20" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="42" t="s">
+    <row r="8" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A8" s="50"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="31"/>
+    </row>
+    <row r="9" spans="1:19" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickTop="1">
+      <c r="A10" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="33"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A11" s="42"/>
-      <c r="B11" s="25" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="44"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="49"/>
+      <c r="B11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="35" t="s">
+      <c r="M11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="O11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="26" t="s">
+      <c r="P11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="Q11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="S11" s="35" t="s">
+      <c r="S11" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="37"/>
-    </row>
-    <row r="13" spans="1:19" s="47" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-    </row>
-    <row r="14" spans="1:19" ht="20" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A12" s="50"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="31"/>
+    </row>
+    <row r="13" spans="1:19" s="35" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="B6:D6"/>
@@ -1760,10 +1757,22 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K10:M10"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>